<commit_message>
Add analysis of C1819-E3
</commit_message>
<xml_diff>
--- a/data/C1819.xlsx
+++ b/data/C1819.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="15540" windowWidth="25520" xWindow="5860" yWindow="1980"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="15540" windowWidth="25520" xWindow="5860" yWindow="1980"/>
   </bookViews>
   <sheets>
     <sheet name="E1" sheetId="1" state="visible" r:id="rId1"/>
@@ -1496,7 +1496,7 @@
   </sheetPr>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2429,10 +2429,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -2494,6 +2494,21 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>35</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.73</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2506,6 +2521,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="H3" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2518,6 +2545,21 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>44</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2530,6 +2572,24 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2542,6 +2602,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="H6" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2554,6 +2626,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>51.7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7.21</v>
+      </c>
+      <c r="H7" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2566,6 +2650,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="H8" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2578,6 +2674,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C9" t="n">
+        <v>85.7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="H9" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2590,6 +2698,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>52.2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="H10" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2602,6 +2722,21 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>28</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2614,6 +2749,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C12" t="n">
+        <v>20</v>
+      </c>
+      <c r="D12" t="n">
+        <v>14.11</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2626,6 +2773,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C13" t="n">
+        <v>68</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="H13" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2638,6 +2797,21 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C14" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="E14" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2650,6 +2824,24 @@
           <t>FPB</t>
         </is>
       </c>
+      <c r="C15" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="E15" t="n">
+        <v>32.31</v>
+      </c>
+      <c r="F15" t="n">
+        <v>5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>6</v>
+      </c>
+      <c r="H15" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2662,6 +2854,18 @@
           <t>FPB</t>
         </is>
       </c>
+      <c r="C16" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8.07</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2674,6 +2878,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C17" t="n">
+        <v>47.6</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="H17" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2686,6 +2902,21 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C18" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2698,6 +2929,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>68.40000000000001</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="H19" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2710,6 +2953,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C20" t="n">
+        <v>72.40000000000001</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="H20" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2722,6 +2977,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C21" t="n">
+        <v>60</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="E21" t="n">
+        <v>18.59</v>
+      </c>
+      <c r="H21" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2734,6 +3001,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5.28</v>
+      </c>
+      <c r="E22" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="H22" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2746,6 +3025,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C23" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E23" t="n">
+        <v>17.49</v>
+      </c>
+      <c r="H23" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2758,6 +3049,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C24" t="n">
+        <v>100</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6.06</v>
+      </c>
+      <c r="H24" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2770,6 +3073,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6.52</v>
+      </c>
+      <c r="H25" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2782,6 +3097,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E26" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="H26" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2794,6 +3121,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C27" t="n">
+        <v>82.40000000000001</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E27" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="H27" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2806,6 +3145,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C28" t="n">
+        <v>85.7</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>8.869999999999999</v>
+      </c>
+      <c r="H28" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2818,6 +3169,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C29" t="n">
+        <v>64</v>
+      </c>
+      <c r="D29" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="E29" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="H29" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2830,6 +3193,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C30" t="n">
+        <v>41.9</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="E30" t="n">
+        <v>13.48</v>
+      </c>
+      <c r="H30" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2842,6 +3217,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C31" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="E31" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="H31" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2854,6 +3241,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C32" t="n">
+        <v>100</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="H32" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2866,6 +3265,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C33" t="n">
+        <v>88.5</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="H33" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2878,6 +3289,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C34" t="n">
+        <v>100</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="E34" t="n">
+        <v>9.73</v>
+      </c>
+      <c r="H34" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2890,6 +3313,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C35" t="n">
+        <v>100</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="H35" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2901,6 +3336,90 @@
         <is>
           <t>CFGS</t>
         </is>
+      </c>
+      <c r="C36" t="n">
+        <v>92.90000000000001</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E36" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="H36" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>1DAM</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CFGS</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="H37" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2DAM</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CFGS</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="H38" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>3DAM</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CFGS</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>84.59999999999999</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H39" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>